<commit_message>
Atualização automática de ERECHIM.xlsx
</commit_message>
<xml_diff>
--- a/ERECHIM.xlsx
+++ b/ERECHIM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00715608-3DF7-4AEE-B3A2-264F67D6CAD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F8480ACD-275B-4EF6-944A-E320556C14CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,20 +23,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="7" r:id="rId8"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="8" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1146,7 +1133,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1207,30 +1194,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -1248,7 +1211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1287,17 +1250,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1343,7 +1301,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{6361EEBA-7F56-4A74-915F-C1CEEDBFEBDC}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{902A6205-B772-40FA-ABF9-286752B16EA9}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1373,10 +1331,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2CDF5E2-8421-4032-9DBD-9A098207BC7E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31B3092E-C5AF-47EF-B156-AC6D34E1967B}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1414,7 +1372,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9675C2F5-B770-430D-BA4B-083A3AAE4389}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{268F5054-A253-42FB-8413-65E747CA5489}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1477,7 +1435,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37CB7E55-23C2-4062-85BF-E63C6DF46483}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED2B7A05-B1E4-42AA-BC07-A4052FA0AD53}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1496,7 +1454,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{31EC09CD-2770-12A0-2DEB-1C085C2678A3}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8908767-1C7B-754C-C6C7-14286CF2776F}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1545,7 +1503,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB9B2D9A-4991-1185-4805-3C19611F20EC}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458DF862-6BF4-B6D3-53CD-B90889DF5DCE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1564,7 +1522,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5FCFE2A-4012-D5AF-B43E-15894209D7B0}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E603286-FF17-4689-9F66-FBC39FAD9CD0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1595,7 +1553,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B80250F1-72C1-5638-D823-63EA8D213FA3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8484BDA9-66D3-3CF9-AFB1-B14091636A21}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1626,7 +1584,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF003EFF-0AB4-1A5B-AB53-12CBA4E3CFB2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAF701B6-C405-7347-D729-075536F5258F}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1669,7 +1627,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8BA3E3E-AA83-4606-9AF5-C0EE1A89C788}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A6141D2-5AED-4553-94C8-F8FCEF8AB279}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1707,7 +1665,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5089C23-2005-49E4-A80C-2269D2505E71}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DA1EC98-299E-4BBD-95E8-C23CC9AE2DE9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1750,7 +1708,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C848CA7-CC8F-41BD-9971-BD8E53337622}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B023EA59-3538-4699-BD7E-B8C7A90DEF4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2063,7 +2021,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EC50F5-DB0A-4E6D-AE9F-A22755BAF325}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{407A0E04-FB87-48D0-AF39-2A63EE5BF903}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2075,98 +2033,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="40"/>
-    <col min="6" max="6" width="2" style="40" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="40" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="40"/>
+    <col min="1" max="5" width="12.5703125" style="37"/>
+    <col min="6" max="6" width="2" style="37" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="37" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="37"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="39"/>
+      <c r="F1" s="36"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="39"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="39"/>
+      <c r="F3" s="36"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="39"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="39"/>
+      <c r="F5" s="36"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="39"/>
+      <c r="F6" s="36"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="39"/>
+      <c r="F7" s="36"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="39"/>
+      <c r="F8" s="36"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="39"/>
+      <c r="F9" s="36"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="39"/>
+      <c r="F10" s="36"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="39"/>
+      <c r="F11" s="36"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="39"/>
+      <c r="F12" s="36"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="39"/>
+      <c r="F13" s="36"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="39"/>
+      <c r="F14" s="36"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="39"/>
+      <c r="F15" s="36"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="39"/>
+      <c r="F16" s="36"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="39"/>
+      <c r="F17" s="36"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="39"/>
+      <c r="F18" s="36"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="39"/>
+      <c r="F19" s="36"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="39"/>
+      <c r="F20" s="36"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="39"/>
+      <c r="F21" s="36"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="39"/>
+      <c r="F22" s="36"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="39"/>
+      <c r="F23" s="36"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="39"/>
+      <c r="F24" s="36"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="39"/>
+      <c r="F25" s="36"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="39"/>
+      <c r="F26" s="36"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="39"/>
+      <c r="F27" s="36"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="39"/>
+      <c r="F28" s="36"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="39"/>
+      <c r="F29" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5400,19 +5358,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5446,46 +5404,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>272</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="17" t="s">
         <v>275</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="17" t="s">
         <v>276</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="17" t="s">
         <v>277</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="17" t="s">
         <v>278</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="17" t="s">
         <v>281</v>
       </c>
     </row>
@@ -5493,7 +5451,7 @@
       <c r="A2" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="22">
+      <c r="B2" s="19">
         <v>462914</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -5505,10 +5463,10 @@
       <c r="E2" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="20">
         <v>275.2</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="20">
         <v>640</v>
       </c>
       <c r="H2" s="2" t="s">
@@ -5537,7 +5495,7 @@
       <c r="A3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B3" s="22">
+      <c r="B3" s="19">
         <v>460413</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -5549,10 +5507,10 @@
       <c r="E3" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="20">
         <v>2784</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="20">
         <v>4800</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -5591,14 +5549,14 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="69.5703125" customWidth="1"/>
+    <col min="2" max="2" width="74.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="17" t="s">
         <v>295</v>
       </c>
     </row>
@@ -5629,79 +5587,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="21" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>298</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>300</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="23" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="23" t="s">
         <v>301</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="23" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="23" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="23" t="s">
         <v>304</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="23" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="23" t="s">
         <v>305</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="23" t="s">
         <v>302</v>
       </c>
     </row>
@@ -5726,54 +5684,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>307</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>309</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>310</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>313</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>316</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>317</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>318</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>319</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>320</v>
       </c>
     </row>
@@ -5784,41 +5743,41 @@
       <c r="B2" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45901</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F2" s="31">
+      <c r="F2" s="28">
         <v>38457</v>
       </c>
-      <c r="G2" s="31">
+      <c r="G2" s="28">
         <v>4986</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="L2" s="32" t="s">
+      <c r="L2" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>325</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="30" t="s">
         <v>325</v>
       </c>
     </row>
@@ -5849,25 +5808,24 @@
       <c r="B1" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="31" t="s">
         <v>327</v>
       </c>
-      <c r="E1" s="35">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="32">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="34" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="35">
         <v>27</v>
       </c>
-      <c r="F1" s="36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
-        <v>282</v>
-      </c>
-      <c r="B2" s="38">
-        <v>27</v>
-      </c>
-      <c r="C2" s="36">
+      <c r="C2" s="33">
         <v>1.785478111360931E-3</v>
       </c>
     </row>

</xml_diff>